<commit_message>
updated the code to run in debugger mode
</commit_message>
<xml_diff>
--- a/src/test/java/projects/trakzee/testCases/web/multiobjectRunning/Object.xlsx
+++ b/src/test/java/projects/trakzee/testCases/web/multiobjectRunning/Object.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t xml:space="preserve">Want To Skip</t>
   </si>
@@ -43,7 +43,10 @@
     <t xml:space="preserve">5</t>
   </si>
   <si>
-    <t xml:space="preserve">1594826005</t>
+    <t xml:space="preserve">1594826001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1594826003</t>
   </si>
 </sst>
 </file>
@@ -177,7 +180,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -231,6 +234,21 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update the code to handle the object and path file from the desktop by adding the new argument in the command second for object path and third for path
</commit_message>
<xml_diff>
--- a/src/test/java/projects/trakzee/testCases/web/multiobjectRunning/Object.xlsx
+++ b/src/test/java/projects/trakzee/testCases/web/multiobjectRunning/Object.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="25">
   <si>
     <t xml:space="preserve">Want To Skip</t>
   </si>
@@ -34,19 +34,67 @@
     <t xml:space="preserve">Time Interval</t>
   </si>
   <si>
+    <t xml:space="preserve">Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1594826001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.127.251.87:5175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trakzee Premium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1594826002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1594826003</t>
+  </si>
+  <si>
     <t xml:space="preserve">1594826004</t>
   </si>
   <si>
+    <t xml:space="preserve">1594826005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1594826006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1594826007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1594826008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1594826009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1594826010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">159482601001</t>
+  </si>
+  <si>
     <t xml:space="preserve">3.7.208.99:5175</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1594826001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1594826003</t>
+    <t xml:space="preserve">QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trakzee Standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">159482601002</t>
   </si>
 </sst>
 </file>
@@ -82,12 +130,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -131,7 +185,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -148,16 +202,32 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -177,20 +247,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1048576"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="17.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.86"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -203,50 +274,326 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="A2" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>6</v>
+      <c r="A3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>6</v>
+      <c r="A4" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B14" s="10" t="n">
+        <v>1594826001</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B15" s="10" t="n">
+        <v>1594826003</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B16" s="10" t="n">
+        <v>1594826004</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
updated the code to handle the server, object and path file and varible data via .ser file, to avoid the error about the server if not passing from the terminal
</commit_message>
<xml_diff>
--- a/src/test/java/projects/trakzee/testCases/web/multiobjectRunning/Object.xlsx
+++ b/src/test/java/projects/trakzee/testCases/web/multiobjectRunning/Object.xlsx
@@ -250,7 +250,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -282,9 +282,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A2" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -303,9 +302,8 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A3" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>11</v>
@@ -324,9 +322,8 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A4" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>12</v>
@@ -345,9 +342,8 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A5" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
@@ -366,9 +362,8 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A6" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>14</v>
@@ -387,9 +382,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A7" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -408,9 +402,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A8" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>16</v>
@@ -429,9 +422,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A9" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>17</v>
@@ -450,9 +442,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A10" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>18</v>
@@ -471,9 +462,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A11" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>19</v>
@@ -492,9 +482,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A12" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>20</v>
@@ -513,9 +502,8 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A13" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>24</v>
@@ -534,9 +522,8 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A14" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="B14" s="10" t="n">
         <v>1594826001</v>

</xml_diff>